<commit_message>
Modified xlsx testing file in 'results/excel': MVP_Flow_Analysis_Test_4
</commit_message>
<xml_diff>
--- a/CriticalFlowPath/results/excel/MVP_Flow_Analysis_Test_4.xlsx
+++ b/CriticalFlowPath/results/excel/MVP_Flow_Analysis_Test_4.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Framework" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Sheet2 " sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Test Dani" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Framework" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -21,7 +22,7 @@
     <numFmt numFmtId="164" formatCode="m"/>
     <numFmt numFmtId="165" formatCode="d"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -70,23 +71,28 @@
     <font>
       <name val="Century Gothic"/>
       <b val="1"/>
-      <color rgb="00FFFFFF"/>
+      <color rgb="FFFFFFFF"/>
       <sz val="12"/>
     </font>
     <font>
       <name val="Century Gothic"/>
       <b val="1"/>
-      <color rgb="00333333"/>
+      <color rgb="FF333333"/>
       <sz val="12"/>
     </font>
     <font>
       <name val="Century Gothic"/>
       <b val="1"/>
-      <color rgb="00000000"/>
+      <color rgb="FF000000"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <name val="Aptos Narrow"/>
+      <b val="1"/>
       <sz val="12"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill/>
     </fill>
@@ -143,36 +149,42 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="008ED973"/>
-        <bgColor rgb="008ED973"/>
+        <fgColor rgb="FF8ED973"/>
+        <bgColor rgb="FF8ED973"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="004D93D9"/>
-        <bgColor rgb="004D93D9"/>
+        <fgColor rgb="FF4D93D9"/>
+        <bgColor rgb="FF4D93D9"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00800080"/>
-        <bgColor rgb="00800080"/>
+        <fgColor rgb="FF800080"/>
+        <bgColor rgb="FF800080"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00CC99FF"/>
-        <bgColor rgb="00CC99FF"/>
+        <fgColor rgb="FFCC99FF"/>
+        <bgColor rgb="FFCC99FF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00C0C0C0"/>
-        <bgColor rgb="00C0C0C0"/>
+        <fgColor rgb="FFC0C0C0"/>
+        <bgColor rgb="FFC0C0C0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -216,15 +228,102 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -267,41 +366,20 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="14" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -313,15 +391,60 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -652,43 +775,49 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AR14"/>
+  <dimension ref="A1:AR27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15.6"/>
+  <cols>
+    <col width="17.546875" bestFit="1" customWidth="1" style="35" min="1" max="1"/>
+    <col width="8.046875" bestFit="1" customWidth="1" style="35" min="2" max="2"/>
+    <col width="12.046875" bestFit="1" customWidth="1" style="35" min="3" max="3"/>
+    <col width="12.69921875" bestFit="1" customWidth="1" style="35" min="4" max="4"/>
+  </cols>
   <sheetData>
-    <row r="1" ht="62.7" customHeight="1">
+    <row r="1" ht="62.7" customHeight="1" s="35">
       <c r="A1" s="4" t="inlineStr">
         <is>
           <t>CPM</t>
         </is>
       </c>
-      <c r="H1" s="19" t="inlineStr">
+      <c r="H1" s="12" t="inlineStr">
         <is>
           <t>2024</t>
         </is>
       </c>
-      <c r="I1" s="24" t="inlineStr">
+      <c r="I1" s="36" t="inlineStr">
         <is>
           <t>2024</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="H2" s="18" t="inlineStr">
+      <c r="H2" s="13" t="inlineStr">
         <is>
           <t>Sep</t>
         </is>
       </c>
-      <c r="I2" s="25" t="inlineStr">
+      <c r="I2" s="34" t="inlineStr">
         <is>
           <t>Sep</t>
         </is>
       </c>
-      <c r="AG2" s="25" t="inlineStr">
+      <c r="AG2" s="34" t="inlineStr">
         <is>
           <t>Oct</t>
         </is>
@@ -2178,11 +2307,188 @@
       <c r="AQ14" s="8" t="n"/>
       <c r="AR14" s="8" t="n"/>
     </row>
+    <row r="17">
+      <c r="A17" s="30" t="inlineStr">
+        <is>
+          <t>phase</t>
+        </is>
+      </c>
+      <c r="B17" s="30" t="inlineStr">
+        <is>
+          <t>trade</t>
+        </is>
+      </c>
+      <c r="C17" s="30" t="inlineStr">
+        <is>
+          <t>activity_code</t>
+        </is>
+      </c>
+      <c r="D17" s="30" t="inlineStr">
+        <is>
+          <t>activity_name</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="37" t="inlineStr">
+        <is>
+          <t>Phase 1</t>
+        </is>
+      </c>
+      <c r="B18" s="38" t="inlineStr">
+        <is>
+          <t>Trade 1</t>
+        </is>
+      </c>
+      <c r="C18" s="31" t="inlineStr">
+        <is>
+          <t>1A</t>
+        </is>
+      </c>
+      <c r="D18" s="31" t="inlineStr">
+        <is>
+          <t>Activity 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="48" t="n"/>
+      <c r="B19" s="48" t="n"/>
+      <c r="C19" s="31" t="inlineStr">
+        <is>
+          <t>1B</t>
+        </is>
+      </c>
+      <c r="D19" s="31" t="inlineStr">
+        <is>
+          <t>Activity 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="48" t="n"/>
+      <c r="B20" s="48" t="n"/>
+      <c r="C20" s="31" t="inlineStr">
+        <is>
+          <t>1C</t>
+        </is>
+      </c>
+      <c r="D20" s="31" t="inlineStr">
+        <is>
+          <t>Activity 3</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="48" t="n"/>
+      <c r="B21" s="48" t="n"/>
+      <c r="C21" s="31" t="inlineStr">
+        <is>
+          <t>1D</t>
+        </is>
+      </c>
+      <c r="D21" s="31" t="inlineStr">
+        <is>
+          <t>Activity 4</t>
+        </is>
+      </c>
+    </row>
+    <row r="22" ht="15.9" customHeight="1" s="35" thickBot="1">
+      <c r="A22" s="48" t="n"/>
+      <c r="B22" s="32" t="n"/>
+      <c r="C22" s="33" t="inlineStr">
+        <is>
+          <t>1E</t>
+        </is>
+      </c>
+      <c r="D22" s="33" t="inlineStr">
+        <is>
+          <t>Activity 5</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="48" t="n"/>
+      <c r="B23" s="40" t="inlineStr">
+        <is>
+          <t>Trade 2</t>
+        </is>
+      </c>
+      <c r="C23" s="32" t="inlineStr">
+        <is>
+          <t>2A</t>
+        </is>
+      </c>
+      <c r="D23" s="32" t="inlineStr">
+        <is>
+          <t>Activity 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="48" t="n"/>
+      <c r="B24" s="48" t="n"/>
+      <c r="C24" s="31" t="inlineStr">
+        <is>
+          <t>2B</t>
+        </is>
+      </c>
+      <c r="D24" s="31" t="inlineStr">
+        <is>
+          <t>Activity 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="48" t="n"/>
+      <c r="B25" s="48" t="n"/>
+      <c r="C25" s="31" t="inlineStr">
+        <is>
+          <t>2C</t>
+        </is>
+      </c>
+      <c r="D25" s="31" t="inlineStr">
+        <is>
+          <t>Activity 3</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="48" t="n"/>
+      <c r="B26" s="48" t="n"/>
+      <c r="C26" s="31" t="inlineStr">
+        <is>
+          <t>2D</t>
+        </is>
+      </c>
+      <c r="D26" s="31" t="inlineStr">
+        <is>
+          <t>Activity 4</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="32" t="n"/>
+      <c r="B27" s="32" t="n"/>
+      <c r="C27" s="31" t="inlineStr">
+        <is>
+          <t>2E</t>
+        </is>
+      </c>
+      <c r="D27" s="31" t="inlineStr">
+        <is>
+          <t>Activity 5</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="I2:AF2"/>
+  <mergeCells count="6">
+    <mergeCell ref="A18:A27"/>
+    <mergeCell ref="B18:B22"/>
     <mergeCell ref="I1:AR1"/>
     <mergeCell ref="AG2:AR2"/>
+    <mergeCell ref="I2:AF2"/>
+    <mergeCell ref="B23:B27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2194,116 +2500,89 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AS14"/>
+  <dimension ref="A1:AS27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+    <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15.6"/>
+  <cols>
+    <col width="8.046875" customWidth="1" style="35" min="2" max="2"/>
+    <col width="12.046875" bestFit="1" customWidth="1" style="35" min="3" max="3"/>
+    <col width="12.69921875" bestFit="1" customWidth="1" style="35" min="4" max="4"/>
+    <col width="5.34765625" bestFit="1" customWidth="1" style="35" min="9" max="9"/>
+    <col width="3.3984375" bestFit="1" customWidth="1" style="35" min="10" max="10"/>
+    <col width="3.84765625" bestFit="1" customWidth="1" style="35" min="11" max="11"/>
+    <col width="4.19921875" bestFit="1" customWidth="1" style="35" min="12" max="12"/>
+    <col width="3.59765625" bestFit="1" customWidth="1" style="35" min="13" max="13"/>
+    <col width="4.3984375" bestFit="1" customWidth="1" style="35" min="14" max="14"/>
+    <col width="3.59765625" bestFit="1" customWidth="1" style="35" min="15" max="15"/>
+    <col width="3.046875" bestFit="1" customWidth="1" style="35" min="16" max="16"/>
+    <col width="3.3984375" bestFit="1" customWidth="1" style="35" min="17" max="17"/>
+    <col width="3.84765625" bestFit="1" customWidth="1" style="35" min="18" max="18"/>
+    <col width="4.19921875" bestFit="1" customWidth="1" style="35" min="19" max="19"/>
+    <col width="3.59765625" bestFit="1" customWidth="1" style="35" min="20" max="20"/>
+    <col width="4.3984375" bestFit="1" customWidth="1" style="35" min="21" max="21"/>
+    <col width="3.59765625" bestFit="1" customWidth="1" style="35" min="22" max="22"/>
+    <col width="3.046875" bestFit="1" customWidth="1" style="35" min="23" max="23"/>
+    <col width="3.3984375" bestFit="1" customWidth="1" style="35" min="24" max="24"/>
+    <col width="3.84765625" bestFit="1" customWidth="1" style="35" min="25" max="25"/>
+    <col width="4.19921875" bestFit="1" customWidth="1" style="35" min="26" max="26"/>
+    <col width="3.59765625" bestFit="1" customWidth="1" style="35" min="27" max="27"/>
+    <col width="4.3984375" bestFit="1" customWidth="1" style="35" min="28" max="28"/>
+    <col width="3.59765625" bestFit="1" customWidth="1" style="35" min="29" max="29"/>
+    <col width="3.046875" bestFit="1" customWidth="1" style="35" min="30" max="30"/>
+    <col width="3.3984375" bestFit="1" customWidth="1" style="35" min="31" max="31"/>
+    <col width="3.84765625" bestFit="1" customWidth="1" style="35" min="32" max="32"/>
+    <col width="4.19921875" bestFit="1" customWidth="1" style="35" min="33" max="33"/>
+    <col width="3.59765625" bestFit="1" customWidth="1" style="35" min="34" max="34"/>
+    <col width="4.3984375" bestFit="1" customWidth="1" style="35" min="35" max="35"/>
+    <col width="3.59765625" bestFit="1" customWidth="1" style="35" min="36" max="36"/>
+    <col width="3.046875" bestFit="1" customWidth="1" style="35" min="37" max="37"/>
+    <col width="3.3984375" bestFit="1" customWidth="1" style="35" min="38" max="38"/>
+    <col width="3.84765625" bestFit="1" customWidth="1" style="35" min="39" max="39"/>
+    <col width="4.19921875" bestFit="1" customWidth="1" style="35" min="40" max="40"/>
+    <col width="3.59765625" bestFit="1" customWidth="1" style="35" min="41" max="41"/>
+    <col width="4.3984375" bestFit="1" customWidth="1" style="35" min="42" max="42"/>
+    <col width="3.59765625" bestFit="1" customWidth="1" style="35" min="43" max="43"/>
+    <col width="3.046875" bestFit="1" customWidth="1" style="35" min="44" max="44"/>
+    <col width="3.3984375" bestFit="1" customWidth="1" style="35" min="45" max="45"/>
+  </cols>
   <sheetData>
-    <row r="1" ht="62.7" customHeight="1">
+    <row r="1" ht="62.7" customHeight="1" s="35">
       <c r="A1" s="4" t="inlineStr">
         <is>
           <t>CPM</t>
         </is>
       </c>
-      <c r="I1" s="29" t="inlineStr">
+      <c r="I1" s="24" t="inlineStr">
         <is>
           <t>2024</t>
         </is>
       </c>
-      <c r="J1" s="30" t="inlineStr">
+      <c r="J1" s="41" t="inlineStr">
         <is>
           <t>2024</t>
         </is>
       </c>
-      <c r="K1" s="29" t="n"/>
-      <c r="L1" s="29" t="n"/>
-      <c r="M1" s="29" t="n"/>
-      <c r="N1" s="29" t="n"/>
-      <c r="O1" s="29" t="n"/>
-      <c r="P1" s="29" t="n"/>
-      <c r="Q1" s="29" t="n"/>
-      <c r="R1" s="29" t="n"/>
-      <c r="S1" s="29" t="n"/>
-      <c r="T1" s="29" t="n"/>
-      <c r="U1" s="29" t="n"/>
-      <c r="V1" s="29" t="n"/>
-      <c r="W1" s="29" t="n"/>
-      <c r="X1" s="29" t="n"/>
-      <c r="Y1" s="29" t="n"/>
-      <c r="Z1" s="29" t="n"/>
-      <c r="AA1" s="29" t="n"/>
-      <c r="AB1" s="29" t="n"/>
-      <c r="AC1" s="29" t="n"/>
-      <c r="AD1" s="29" t="n"/>
-      <c r="AE1" s="29" t="n"/>
-      <c r="AF1" s="29" t="n"/>
-      <c r="AG1" s="29" t="n"/>
-      <c r="AH1" s="29" t="n"/>
-      <c r="AI1" s="29" t="n"/>
-      <c r="AJ1" s="29" t="n"/>
-      <c r="AK1" s="29" t="n"/>
-      <c r="AL1" s="29" t="n"/>
-      <c r="AM1" s="29" t="n"/>
-      <c r="AN1" s="29" t="n"/>
-      <c r="AO1" s="29" t="n"/>
-      <c r="AP1" s="29" t="n"/>
-      <c r="AQ1" s="29" t="n"/>
-      <c r="AR1" s="29" t="n"/>
-      <c r="AS1" s="29" t="n"/>
     </row>
     <row r="2">
-      <c r="I2" s="31" t="inlineStr">
+      <c r="I2" s="25" t="inlineStr">
         <is>
           <t>Sep</t>
         </is>
       </c>
-      <c r="J2" s="32" t="inlineStr">
+      <c r="J2" s="42" t="inlineStr">
         <is>
           <t>Sep</t>
         </is>
       </c>
-      <c r="K2" s="31" t="n"/>
-      <c r="L2" s="31" t="n"/>
-      <c r="M2" s="31" t="n"/>
-      <c r="N2" s="31" t="n"/>
-      <c r="O2" s="31" t="n"/>
-      <c r="P2" s="31" t="n"/>
-      <c r="Q2" s="31" t="n"/>
-      <c r="R2" s="31" t="n"/>
-      <c r="S2" s="31" t="n"/>
-      <c r="T2" s="31" t="n"/>
-      <c r="U2" s="31" t="n"/>
-      <c r="V2" s="31" t="n"/>
-      <c r="W2" s="31" t="n"/>
-      <c r="X2" s="31" t="n"/>
-      <c r="Y2" s="31" t="n"/>
-      <c r="Z2" s="31" t="n"/>
-      <c r="AA2" s="31" t="n"/>
-      <c r="AB2" s="31" t="n"/>
-      <c r="AC2" s="31" t="n"/>
-      <c r="AD2" s="31" t="n"/>
-      <c r="AE2" s="31" t="n"/>
-      <c r="AF2" s="31" t="n"/>
-      <c r="AG2" s="31" t="n"/>
-      <c r="AH2" s="32" t="inlineStr">
+      <c r="AH2" s="42" t="inlineStr">
         <is>
           <t>Oct</t>
         </is>
       </c>
-      <c r="AI2" s="31" t="n"/>
-      <c r="AJ2" s="31" t="n"/>
-      <c r="AK2" s="31" t="n"/>
-      <c r="AL2" s="31" t="n"/>
-      <c r="AM2" s="31" t="n"/>
-      <c r="AN2" s="31" t="n"/>
-      <c r="AO2" s="31" t="n"/>
-      <c r="AP2" s="31" t="n"/>
-      <c r="AQ2" s="31" t="n"/>
-      <c r="AR2" s="31" t="n"/>
-      <c r="AS2" s="31" t="n"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -2341,187 +2620,187 @@
           <t>PM</t>
         </is>
       </c>
-      <c r="I3" s="33" t="inlineStr">
+      <c r="I3" s="26" t="inlineStr">
         <is>
           <t>06</t>
         </is>
       </c>
-      <c r="J3" s="33" t="inlineStr">
+      <c r="J3" s="26" t="inlineStr">
         <is>
           <t>07</t>
         </is>
       </c>
-      <c r="K3" s="34" t="inlineStr">
+      <c r="K3" s="27" t="inlineStr">
         <is>
           <t>08</t>
         </is>
       </c>
-      <c r="L3" s="34" t="inlineStr">
+      <c r="L3" s="27" t="inlineStr">
         <is>
           <t>09</t>
         </is>
       </c>
-      <c r="M3" s="34" t="inlineStr">
+      <c r="M3" s="27" t="inlineStr">
         <is>
           <t>10</t>
         </is>
       </c>
-      <c r="N3" s="34" t="inlineStr">
+      <c r="N3" s="27" t="inlineStr">
         <is>
           <t>11</t>
         </is>
       </c>
-      <c r="O3" s="34" t="inlineStr">
+      <c r="O3" s="27" t="inlineStr">
         <is>
           <t>12</t>
         </is>
       </c>
-      <c r="P3" s="34" t="inlineStr">
+      <c r="P3" s="27" t="inlineStr">
         <is>
           <t>13</t>
         </is>
       </c>
-      <c r="Q3" s="34" t="inlineStr">
+      <c r="Q3" s="27" t="inlineStr">
         <is>
           <t>14</t>
         </is>
       </c>
-      <c r="R3" s="34" t="inlineStr">
+      <c r="R3" s="27" t="inlineStr">
         <is>
           <t>15</t>
         </is>
       </c>
-      <c r="S3" s="34" t="inlineStr">
+      <c r="S3" s="27" t="inlineStr">
         <is>
           <t>16</t>
         </is>
       </c>
-      <c r="T3" s="34" t="inlineStr">
+      <c r="T3" s="27" t="inlineStr">
         <is>
           <t>17</t>
         </is>
       </c>
-      <c r="U3" s="34" t="inlineStr">
+      <c r="U3" s="27" t="inlineStr">
         <is>
           <t>18</t>
         </is>
       </c>
-      <c r="V3" s="34" t="inlineStr">
+      <c r="V3" s="27" t="inlineStr">
         <is>
           <t>19</t>
         </is>
       </c>
-      <c r="W3" s="34" t="inlineStr">
+      <c r="W3" s="27" t="inlineStr">
         <is>
           <t>20</t>
         </is>
       </c>
-      <c r="X3" s="34" t="inlineStr">
+      <c r="X3" s="27" t="inlineStr">
         <is>
           <t>21</t>
         </is>
       </c>
-      <c r="Y3" s="34" t="inlineStr">
+      <c r="Y3" s="27" t="inlineStr">
         <is>
           <t>22</t>
         </is>
       </c>
-      <c r="Z3" s="34" t="inlineStr">
+      <c r="Z3" s="27" t="inlineStr">
         <is>
           <t>23</t>
         </is>
       </c>
-      <c r="AA3" s="34" t="inlineStr">
+      <c r="AA3" s="27" t="inlineStr">
         <is>
           <t>24</t>
         </is>
       </c>
-      <c r="AB3" s="34" t="inlineStr">
+      <c r="AB3" s="27" t="inlineStr">
         <is>
           <t>25</t>
         </is>
       </c>
-      <c r="AC3" s="34" t="inlineStr">
+      <c r="AC3" s="27" t="inlineStr">
         <is>
           <t>26</t>
         </is>
       </c>
-      <c r="AD3" s="34" t="inlineStr">
+      <c r="AD3" s="27" t="inlineStr">
         <is>
           <t>27</t>
         </is>
       </c>
-      <c r="AE3" s="34" t="inlineStr">
+      <c r="AE3" s="27" t="inlineStr">
         <is>
           <t>28</t>
         </is>
       </c>
-      <c r="AF3" s="34" t="inlineStr">
+      <c r="AF3" s="27" t="inlineStr">
         <is>
           <t>29</t>
         </is>
       </c>
-      <c r="AG3" s="34" t="inlineStr">
+      <c r="AG3" s="27" t="inlineStr">
         <is>
           <t>30</t>
         </is>
       </c>
-      <c r="AH3" s="33" t="inlineStr">
+      <c r="AH3" s="26" t="inlineStr">
         <is>
           <t>01</t>
         </is>
       </c>
-      <c r="AI3" s="34" t="inlineStr">
+      <c r="AI3" s="27" t="inlineStr">
         <is>
           <t>02</t>
         </is>
       </c>
-      <c r="AJ3" s="34" t="inlineStr">
+      <c r="AJ3" s="27" t="inlineStr">
         <is>
           <t>03</t>
         </is>
       </c>
-      <c r="AK3" s="34" t="inlineStr">
+      <c r="AK3" s="27" t="inlineStr">
         <is>
           <t>04</t>
         </is>
       </c>
-      <c r="AL3" s="34" t="inlineStr">
+      <c r="AL3" s="27" t="inlineStr">
         <is>
           <t>05</t>
         </is>
       </c>
-      <c r="AM3" s="34" t="inlineStr">
+      <c r="AM3" s="27" t="inlineStr">
         <is>
           <t>06</t>
         </is>
       </c>
-      <c r="AN3" s="34" t="inlineStr">
+      <c r="AN3" s="27" t="inlineStr">
         <is>
           <t>07</t>
         </is>
       </c>
-      <c r="AO3" s="34" t="inlineStr">
+      <c r="AO3" s="27" t="inlineStr">
         <is>
           <t>08</t>
         </is>
       </c>
-      <c r="AP3" s="34" t="inlineStr">
+      <c r="AP3" s="27" t="inlineStr">
         <is>
           <t>09</t>
         </is>
       </c>
-      <c r="AQ3" s="34" t="inlineStr">
+      <c r="AQ3" s="27" t="inlineStr">
         <is>
           <t>10</t>
         </is>
       </c>
-      <c r="AR3" s="34" t="inlineStr">
+      <c r="AR3" s="27" t="inlineStr">
         <is>
           <t>11</t>
         </is>
       </c>
-      <c r="AS3" s="34" t="inlineStr">
+      <c r="AS3" s="27" t="inlineStr">
         <is>
           <t>12</t>
         </is>
@@ -2568,12 +2847,12 @@
           <t>Finish</t>
         </is>
       </c>
-      <c r="I4" s="35" t="inlineStr">
+      <c r="I4" s="28" t="inlineStr">
         <is>
           <t>Fri</t>
         </is>
       </c>
-      <c r="J4" s="35" t="inlineStr">
+      <c r="J4" s="28" t="inlineStr">
         <is>
           <t>Sat</t>
         </is>
@@ -2693,7 +2972,7 @@
           <t>Mon</t>
         </is>
       </c>
-      <c r="AH4" s="35" t="inlineStr">
+      <c r="AH4" s="28" t="inlineStr">
         <is>
           <t>Tue</t>
         </is>
@@ -2770,7 +3049,7 @@
           <t>Trade 1</t>
         </is>
       </c>
-      <c r="D5" s="22" t="inlineStr">
+      <c r="D5" s="20" t="inlineStr">
         <is>
           <t>#8ED973</t>
         </is>
@@ -2795,77 +3074,77 @@
           <t>20-Sep-24</t>
         </is>
       </c>
-      <c r="I5" s="36" t="inlineStr">
+      <c r="I5" s="22" t="inlineStr">
         <is>
           <t>1A</t>
         </is>
       </c>
-      <c r="J5" s="36" t="inlineStr">
+      <c r="J5" s="22" t="inlineStr">
         <is>
           <t>1A</t>
         </is>
       </c>
-      <c r="K5" s="37" t="inlineStr">
+      <c r="K5" s="29" t="inlineStr">
         <is>
           <t>1A</t>
         </is>
       </c>
-      <c r="L5" s="37" t="inlineStr">
+      <c r="L5" s="29" t="inlineStr">
         <is>
           <t>1A</t>
         </is>
       </c>
-      <c r="M5" s="37" t="inlineStr">
+      <c r="M5" s="29" t="inlineStr">
         <is>
           <t>1A</t>
         </is>
       </c>
-      <c r="N5" s="37" t="inlineStr">
+      <c r="N5" s="29" t="inlineStr">
         <is>
           <t>1A</t>
         </is>
       </c>
-      <c r="O5" s="37" t="inlineStr">
+      <c r="O5" s="29" t="inlineStr">
         <is>
           <t>1A</t>
         </is>
       </c>
-      <c r="P5" s="37" t="inlineStr">
+      <c r="P5" s="29" t="inlineStr">
         <is>
           <t>1A</t>
         </is>
       </c>
-      <c r="Q5" s="37" t="inlineStr">
+      <c r="Q5" s="29" t="inlineStr">
         <is>
           <t>1A</t>
         </is>
       </c>
-      <c r="R5" s="37" t="inlineStr">
+      <c r="R5" s="29" t="inlineStr">
         <is>
           <t>1A</t>
         </is>
       </c>
-      <c r="S5" s="37" t="inlineStr">
+      <c r="S5" s="29" t="inlineStr">
         <is>
           <t>1A</t>
         </is>
       </c>
-      <c r="T5" s="37" t="inlineStr">
+      <c r="T5" s="29" t="inlineStr">
         <is>
           <t>1A</t>
         </is>
       </c>
-      <c r="U5" s="37" t="inlineStr">
+      <c r="U5" s="29" t="inlineStr">
         <is>
           <t>1A</t>
         </is>
       </c>
-      <c r="V5" s="37" t="inlineStr">
+      <c r="V5" s="29" t="inlineStr">
         <is>
           <t>1A</t>
         </is>
       </c>
-      <c r="W5" s="37" t="inlineStr">
+      <c r="W5" s="29" t="inlineStr">
         <is>
           <t>1A</t>
         </is>
@@ -2879,63 +3158,63 @@
       <c r="AD5" s="8" t="n"/>
       <c r="AE5" s="8" t="n"/>
       <c r="AF5" s="8" t="n"/>
-      <c r="AG5" s="37" t="inlineStr">
+      <c r="AG5" s="29" t="inlineStr">
         <is>
           <t>1B</t>
         </is>
       </c>
-      <c r="AH5" s="36" t="inlineStr">
+      <c r="AH5" s="22" t="inlineStr">
         <is>
           <t>1B</t>
         </is>
       </c>
-      <c r="AI5" s="37" t="inlineStr">
+      <c r="AI5" s="29" t="inlineStr">
         <is>
           <t>1B</t>
         </is>
       </c>
-      <c r="AJ5" s="37" t="inlineStr">
+      <c r="AJ5" s="29" t="inlineStr">
         <is>
           <t>1B</t>
         </is>
       </c>
-      <c r="AK5" s="37" t="inlineStr">
+      <c r="AK5" s="29" t="inlineStr">
         <is>
           <t>1B</t>
         </is>
       </c>
-      <c r="AL5" s="37" t="inlineStr">
+      <c r="AL5" s="29" t="inlineStr">
         <is>
           <t>1B</t>
         </is>
       </c>
       <c r="AM5" s="8" t="n"/>
-      <c r="AN5" s="37" t="inlineStr">
+      <c r="AN5" s="29" t="inlineStr">
         <is>
           <t>1E</t>
         </is>
       </c>
-      <c r="AO5" s="37" t="inlineStr">
+      <c r="AO5" s="29" t="inlineStr">
         <is>
           <t>1E</t>
         </is>
       </c>
-      <c r="AP5" s="37" t="inlineStr">
+      <c r="AP5" s="29" t="inlineStr">
         <is>
           <t>1E</t>
         </is>
       </c>
-      <c r="AQ5" s="37" t="inlineStr">
+      <c r="AQ5" s="29" t="inlineStr">
         <is>
           <t>1E</t>
         </is>
       </c>
-      <c r="AR5" s="37" t="inlineStr">
+      <c r="AR5" s="29" t="inlineStr">
         <is>
           <t>1E</t>
         </is>
       </c>
-      <c r="AS5" s="37" t="inlineStr">
+      <c r="AS5" s="29" t="inlineStr">
         <is>
           <t>1E</t>
         </is>
@@ -2957,7 +3236,7 @@
           <t>Trade 2</t>
         </is>
       </c>
-      <c r="D6" s="23" t="inlineStr">
+      <c r="D6" s="21" t="inlineStr">
         <is>
           <t>#4D93D9</t>
         </is>
@@ -2982,159 +3261,159 @@
           <t>15-Sep-24</t>
         </is>
       </c>
-      <c r="I6" s="35" t="n"/>
-      <c r="J6" s="35" t="n"/>
+      <c r="I6" s="28" t="n"/>
+      <c r="J6" s="28" t="n"/>
       <c r="K6" s="8" t="n"/>
-      <c r="L6" s="38" t="inlineStr">
+      <c r="L6" s="23" t="inlineStr">
         <is>
           <t>2A</t>
         </is>
       </c>
-      <c r="M6" s="38" t="inlineStr">
+      <c r="M6" s="23" t="inlineStr">
         <is>
           <t>2A</t>
         </is>
       </c>
-      <c r="N6" s="38" t="inlineStr">
+      <c r="N6" s="23" t="inlineStr">
         <is>
           <t>2A</t>
         </is>
       </c>
-      <c r="O6" s="38" t="inlineStr">
+      <c r="O6" s="23" t="inlineStr">
         <is>
           <t>2A</t>
         </is>
       </c>
-      <c r="P6" s="38" t="inlineStr">
+      <c r="P6" s="23" t="inlineStr">
         <is>
           <t>2A</t>
         </is>
       </c>
-      <c r="Q6" s="38" t="inlineStr">
+      <c r="Q6" s="23" t="inlineStr">
         <is>
           <t>2A</t>
         </is>
       </c>
-      <c r="R6" s="38" t="inlineStr">
+      <c r="R6" s="23" t="inlineStr">
         <is>
           <t>2A</t>
         </is>
       </c>
-      <c r="S6" s="38" t="inlineStr">
+      <c r="S6" s="23" t="inlineStr">
         <is>
           <t>2B</t>
         </is>
       </c>
-      <c r="T6" s="38" t="inlineStr">
+      <c r="T6" s="23" t="inlineStr">
         <is>
           <t>2B</t>
         </is>
       </c>
-      <c r="U6" s="38" t="inlineStr">
+      <c r="U6" s="23" t="inlineStr">
         <is>
           <t>2B</t>
         </is>
       </c>
-      <c r="V6" s="38" t="inlineStr">
+      <c r="V6" s="23" t="inlineStr">
         <is>
           <t>2B</t>
         </is>
       </c>
-      <c r="W6" s="37" t="inlineStr">
+      <c r="W6" s="29" t="inlineStr">
         <is>
           <t>1C</t>
         </is>
       </c>
-      <c r="X6" s="37" t="inlineStr">
+      <c r="X6" s="29" t="inlineStr">
         <is>
           <t>1C</t>
         </is>
       </c>
-      <c r="Y6" s="37" t="inlineStr">
+      <c r="Y6" s="29" t="inlineStr">
         <is>
           <t>1C</t>
         </is>
       </c>
-      <c r="Z6" s="37" t="inlineStr">
+      <c r="Z6" s="29" t="inlineStr">
         <is>
           <t>1C</t>
         </is>
       </c>
-      <c r="AA6" s="37" t="inlineStr">
+      <c r="AA6" s="29" t="inlineStr">
         <is>
           <t>1C</t>
         </is>
       </c>
-      <c r="AB6" s="37" t="inlineStr">
+      <c r="AB6" s="29" t="inlineStr">
         <is>
           <t>1C</t>
         </is>
       </c>
-      <c r="AC6" s="37" t="inlineStr">
+      <c r="AC6" s="29" t="inlineStr">
         <is>
           <t>1C</t>
         </is>
       </c>
-      <c r="AD6" s="37" t="inlineStr">
+      <c r="AD6" s="29" t="inlineStr">
         <is>
           <t>1C</t>
         </is>
       </c>
-      <c r="AE6" s="37" t="inlineStr">
+      <c r="AE6" s="29" t="inlineStr">
         <is>
           <t>1C</t>
         </is>
       </c>
-      <c r="AF6" s="37" t="inlineStr">
+      <c r="AF6" s="29" t="inlineStr">
         <is>
           <t>1C</t>
         </is>
       </c>
-      <c r="AG6" s="37" t="inlineStr">
+      <c r="AG6" s="29" t="inlineStr">
         <is>
           <t>1C</t>
         </is>
       </c>
-      <c r="AH6" s="35" t="n"/>
+      <c r="AH6" s="28" t="n"/>
       <c r="AI6" s="8" t="n"/>
       <c r="AJ6" s="8" t="n"/>
       <c r="AK6" s="8" t="n"/>
-      <c r="AL6" s="38" t="inlineStr">
+      <c r="AL6" s="23" t="inlineStr">
         <is>
           <t>2C</t>
         </is>
       </c>
-      <c r="AM6" s="38" t="inlineStr">
+      <c r="AM6" s="23" t="inlineStr">
         <is>
           <t>2C</t>
         </is>
       </c>
-      <c r="AN6" s="38" t="inlineStr">
+      <c r="AN6" s="23" t="inlineStr">
         <is>
           <t>2C</t>
         </is>
       </c>
-      <c r="AO6" s="38" t="inlineStr">
+      <c r="AO6" s="23" t="inlineStr">
         <is>
           <t>2C</t>
         </is>
       </c>
-      <c r="AP6" s="38" t="inlineStr">
+      <c r="AP6" s="23" t="inlineStr">
         <is>
           <t>2C</t>
         </is>
       </c>
-      <c r="AQ6" s="38" t="inlineStr">
+      <c r="AQ6" s="23" t="inlineStr">
         <is>
           <t>2E</t>
         </is>
       </c>
-      <c r="AR6" s="38" t="inlineStr">
+      <c r="AR6" s="23" t="inlineStr">
         <is>
           <t>2E</t>
         </is>
       </c>
-      <c r="AS6" s="38" t="inlineStr">
+      <c r="AS6" s="23" t="inlineStr">
         <is>
           <t>2E</t>
         </is>
@@ -3156,7 +3435,7 @@
           <t>Trade 1</t>
         </is>
       </c>
-      <c r="D7" s="22" t="inlineStr">
+      <c r="D7" s="20" t="inlineStr">
         <is>
           <t>#8ED973</t>
         </is>
@@ -3181,8 +3460,8 @@
           <t>5-Oct-24</t>
         </is>
       </c>
-      <c r="I7" s="35" t="n"/>
-      <c r="J7" s="35" t="n"/>
+      <c r="I7" s="28" t="n"/>
+      <c r="J7" s="28" t="n"/>
       <c r="K7" s="8" t="n"/>
       <c r="L7" s="8" t="n"/>
       <c r="M7" s="8" t="n"/>
@@ -3203,77 +3482,77 @@
       <c r="AB7" s="8" t="n"/>
       <c r="AC7" s="8" t="n"/>
       <c r="AD7" s="8" t="n"/>
-      <c r="AE7" s="37" t="inlineStr">
+      <c r="AE7" s="29" t="inlineStr">
         <is>
           <t>1D</t>
         </is>
       </c>
-      <c r="AF7" s="37" t="inlineStr">
+      <c r="AF7" s="29" t="inlineStr">
         <is>
           <t>1D</t>
         </is>
       </c>
-      <c r="AG7" s="37" t="inlineStr">
+      <c r="AG7" s="29" t="inlineStr">
         <is>
           <t>1D</t>
         </is>
       </c>
-      <c r="AH7" s="36" t="inlineStr">
+      <c r="AH7" s="22" t="inlineStr">
         <is>
           <t>1D</t>
         </is>
       </c>
-      <c r="AI7" s="37" t="inlineStr">
+      <c r="AI7" s="29" t="inlineStr">
         <is>
           <t>1D</t>
         </is>
       </c>
-      <c r="AJ7" s="37" t="inlineStr">
+      <c r="AJ7" s="29" t="inlineStr">
         <is>
           <t>1D</t>
         </is>
       </c>
-      <c r="AK7" s="37" t="inlineStr">
+      <c r="AK7" s="29" t="inlineStr">
         <is>
           <t>1D</t>
         </is>
       </c>
-      <c r="AL7" s="37" t="inlineStr">
+      <c r="AL7" s="29" t="inlineStr">
         <is>
           <t>1D</t>
         </is>
       </c>
-      <c r="AM7" s="37" t="inlineStr">
+      <c r="AM7" s="29" t="inlineStr">
         <is>
           <t>1D</t>
         </is>
       </c>
-      <c r="AN7" s="37" t="inlineStr">
+      <c r="AN7" s="29" t="inlineStr">
         <is>
           <t>1D</t>
         </is>
       </c>
-      <c r="AO7" s="37" t="inlineStr">
+      <c r="AO7" s="29" t="inlineStr">
         <is>
           <t>1D</t>
         </is>
       </c>
-      <c r="AP7" s="37" t="inlineStr">
+      <c r="AP7" s="29" t="inlineStr">
         <is>
           <t>1D</t>
         </is>
       </c>
-      <c r="AQ7" s="37" t="inlineStr">
+      <c r="AQ7" s="29" t="inlineStr">
         <is>
           <t>1D</t>
         </is>
       </c>
-      <c r="AR7" s="37" t="inlineStr">
+      <c r="AR7" s="29" t="inlineStr">
         <is>
           <t>1D</t>
         </is>
       </c>
-      <c r="AS7" s="37" t="inlineStr">
+      <c r="AS7" s="29" t="inlineStr">
         <is>
           <t>1D</t>
         </is>
@@ -3295,7 +3574,7 @@
           <t>Trade 2</t>
         </is>
       </c>
-      <c r="D8" s="23" t="inlineStr">
+      <c r="D8" s="21" t="inlineStr">
         <is>
           <t>#4D93D9</t>
         </is>
@@ -3320,8 +3599,8 @@
           <t>19-Sep-24</t>
         </is>
       </c>
-      <c r="I8" s="35" t="n"/>
-      <c r="J8" s="35" t="n"/>
+      <c r="I8" s="28" t="n"/>
+      <c r="J8" s="28" t="n"/>
       <c r="K8" s="8" t="n"/>
       <c r="L8" s="8" t="n"/>
       <c r="M8" s="8" t="n"/>
@@ -3345,21 +3624,21 @@
       <c r="AE8" s="8" t="n"/>
       <c r="AF8" s="8" t="n"/>
       <c r="AG8" s="8" t="n"/>
-      <c r="AH8" s="35" t="n"/>
+      <c r="AH8" s="28" t="n"/>
       <c r="AI8" s="8" t="n"/>
       <c r="AJ8" s="8" t="n"/>
       <c r="AK8" s="8" t="n"/>
-      <c r="AL8" s="38" t="inlineStr">
+      <c r="AL8" s="23" t="inlineStr">
         <is>
           <t>2D</t>
         </is>
       </c>
-      <c r="AM8" s="38" t="inlineStr">
+      <c r="AM8" s="23" t="inlineStr">
         <is>
           <t>2D</t>
         </is>
       </c>
-      <c r="AN8" s="38" t="inlineStr">
+      <c r="AN8" s="23" t="inlineStr">
         <is>
           <t>2D</t>
         </is>
@@ -3386,7 +3665,7 @@
           <t>Trade 1</t>
         </is>
       </c>
-      <c r="D9" s="22" t="inlineStr">
+      <c r="D9" s="20" t="inlineStr">
         <is>
           <t>#8ED973</t>
         </is>
@@ -3411,8 +3690,8 @@
           <t>30-Sep-24</t>
         </is>
       </c>
-      <c r="I9" s="35" t="n"/>
-      <c r="J9" s="35" t="n"/>
+      <c r="I9" s="28" t="n"/>
+      <c r="J9" s="28" t="n"/>
       <c r="K9" s="8" t="n"/>
       <c r="L9" s="8" t="n"/>
       <c r="M9" s="8" t="n"/>
@@ -3436,7 +3715,7 @@
       <c r="AE9" s="8" t="n"/>
       <c r="AF9" s="8" t="n"/>
       <c r="AG9" s="8" t="n"/>
-      <c r="AH9" s="35" t="n"/>
+      <c r="AH9" s="28" t="n"/>
       <c r="AI9" s="8" t="n"/>
       <c r="AJ9" s="8" t="n"/>
       <c r="AK9" s="8" t="n"/>
@@ -3465,7 +3744,7 @@
           <t>Trade 2</t>
         </is>
       </c>
-      <c r="D10" s="23" t="inlineStr">
+      <c r="D10" s="21" t="inlineStr">
         <is>
           <t>#4D93D9</t>
         </is>
@@ -3490,8 +3769,8 @@
           <t>9-Oct-24</t>
         </is>
       </c>
-      <c r="I10" s="35" t="n"/>
-      <c r="J10" s="35" t="n"/>
+      <c r="I10" s="28" t="n"/>
+      <c r="J10" s="28" t="n"/>
       <c r="K10" s="8" t="n"/>
       <c r="L10" s="8" t="n"/>
       <c r="M10" s="8" t="n"/>
@@ -3515,7 +3794,7 @@
       <c r="AE10" s="8" t="n"/>
       <c r="AF10" s="8" t="n"/>
       <c r="AG10" s="8" t="n"/>
-      <c r="AH10" s="35" t="n"/>
+      <c r="AH10" s="28" t="n"/>
       <c r="AI10" s="8" t="n"/>
       <c r="AJ10" s="8" t="n"/>
       <c r="AK10" s="8" t="n"/>
@@ -3544,7 +3823,7 @@
           <t>Trade 1</t>
         </is>
       </c>
-      <c r="D11" s="22" t="inlineStr">
+      <c r="D11" s="20" t="inlineStr">
         <is>
           <t>#8ED973</t>
         </is>
@@ -3569,8 +3848,8 @@
           <t>12-Oct-24</t>
         </is>
       </c>
-      <c r="I11" s="35" t="n"/>
-      <c r="J11" s="35" t="n"/>
+      <c r="I11" s="28" t="n"/>
+      <c r="J11" s="28" t="n"/>
       <c r="K11" s="8" t="n"/>
       <c r="L11" s="8" t="n"/>
       <c r="M11" s="8" t="n"/>
@@ -3594,7 +3873,7 @@
       <c r="AE11" s="8" t="n"/>
       <c r="AF11" s="8" t="n"/>
       <c r="AG11" s="8" t="n"/>
-      <c r="AH11" s="35" t="n"/>
+      <c r="AH11" s="28" t="n"/>
       <c r="AI11" s="8" t="n"/>
       <c r="AJ11" s="8" t="n"/>
       <c r="AK11" s="8" t="n"/>
@@ -3623,7 +3902,7 @@
           <t>Trade 2</t>
         </is>
       </c>
-      <c r="D12" s="23" t="inlineStr">
+      <c r="D12" s="21" t="inlineStr">
         <is>
           <t>#4D93D9</t>
         </is>
@@ -3648,8 +3927,8 @@
           <t>7-Oct-24</t>
         </is>
       </c>
-      <c r="I12" s="35" t="n"/>
-      <c r="J12" s="35" t="n"/>
+      <c r="I12" s="28" t="n"/>
+      <c r="J12" s="28" t="n"/>
       <c r="K12" s="8" t="n"/>
       <c r="L12" s="8" t="n"/>
       <c r="M12" s="8" t="n"/>
@@ -3673,7 +3952,7 @@
       <c r="AE12" s="8" t="n"/>
       <c r="AF12" s="8" t="n"/>
       <c r="AG12" s="8" t="n"/>
-      <c r="AH12" s="35" t="n"/>
+      <c r="AH12" s="28" t="n"/>
       <c r="AI12" s="8" t="n"/>
       <c r="AJ12" s="8" t="n"/>
       <c r="AK12" s="8" t="n"/>
@@ -3702,7 +3981,7 @@
           <t>Trade 1</t>
         </is>
       </c>
-      <c r="D13" s="22" t="inlineStr">
+      <c r="D13" s="20" t="inlineStr">
         <is>
           <t>#8ED973</t>
         </is>
@@ -3727,8 +4006,8 @@
           <t>12-Oct-24</t>
         </is>
       </c>
-      <c r="I13" s="35" t="n"/>
-      <c r="J13" s="35" t="n"/>
+      <c r="I13" s="28" t="n"/>
+      <c r="J13" s="28" t="n"/>
       <c r="K13" s="8" t="n"/>
       <c r="L13" s="8" t="n"/>
       <c r="M13" s="8" t="n"/>
@@ -3752,7 +4031,7 @@
       <c r="AE13" s="8" t="n"/>
       <c r="AF13" s="8" t="n"/>
       <c r="AG13" s="8" t="n"/>
-      <c r="AH13" s="35" t="n"/>
+      <c r="AH13" s="28" t="n"/>
       <c r="AI13" s="8" t="n"/>
       <c r="AJ13" s="8" t="n"/>
       <c r="AK13" s="8" t="n"/>
@@ -3781,7 +4060,7 @@
           <t>Trade 2</t>
         </is>
       </c>
-      <c r="D14" s="23" t="inlineStr">
+      <c r="D14" s="21" t="inlineStr">
         <is>
           <t>#4D93D9</t>
         </is>
@@ -3806,8 +4085,8 @@
           <t>12-Oct-24</t>
         </is>
       </c>
-      <c r="I14" s="35" t="n"/>
-      <c r="J14" s="35" t="n"/>
+      <c r="I14" s="28" t="n"/>
+      <c r="J14" s="28" t="n"/>
       <c r="K14" s="8" t="n"/>
       <c r="L14" s="8" t="n"/>
       <c r="M14" s="8" t="n"/>
@@ -3831,7 +4110,7 @@
       <c r="AE14" s="8" t="n"/>
       <c r="AF14" s="8" t="n"/>
       <c r="AG14" s="8" t="n"/>
-      <c r="AH14" s="35" t="n"/>
+      <c r="AH14" s="28" t="n"/>
       <c r="AI14" s="8" t="n"/>
       <c r="AJ14" s="8" t="n"/>
       <c r="AK14" s="8" t="n"/>
@@ -3844,11 +4123,188 @@
       <c r="AR14" s="8" t="n"/>
       <c r="AS14" s="8" t="n"/>
     </row>
+    <row r="17">
+      <c r="A17" s="30" t="inlineStr">
+        <is>
+          <t>phase</t>
+        </is>
+      </c>
+      <c r="B17" s="30" t="inlineStr">
+        <is>
+          <t>trade</t>
+        </is>
+      </c>
+      <c r="C17" s="30" t="inlineStr">
+        <is>
+          <t>activity_code</t>
+        </is>
+      </c>
+      <c r="D17" s="30" t="inlineStr">
+        <is>
+          <t>activity_name</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="37" t="inlineStr">
+        <is>
+          <t>Phase 1</t>
+        </is>
+      </c>
+      <c r="B18" s="49" t="inlineStr">
+        <is>
+          <t>Trade 1</t>
+        </is>
+      </c>
+      <c r="C18" s="31" t="inlineStr">
+        <is>
+          <t>1A</t>
+        </is>
+      </c>
+      <c r="D18" s="31" t="inlineStr">
+        <is>
+          <t>Activity 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="48" t="n"/>
+      <c r="B19" s="48" t="n"/>
+      <c r="C19" s="31" t="inlineStr">
+        <is>
+          <t>1B</t>
+        </is>
+      </c>
+      <c r="D19" s="31" t="inlineStr">
+        <is>
+          <t>Activity 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="48" t="n"/>
+      <c r="B20" s="48" t="n"/>
+      <c r="C20" s="31" t="inlineStr">
+        <is>
+          <t>1C</t>
+        </is>
+      </c>
+      <c r="D20" s="31" t="inlineStr">
+        <is>
+          <t>Activity 3</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="48" t="n"/>
+      <c r="B21" s="48" t="n"/>
+      <c r="C21" s="31" t="inlineStr">
+        <is>
+          <t>1D</t>
+        </is>
+      </c>
+      <c r="D21" s="31" t="inlineStr">
+        <is>
+          <t>Activity 4</t>
+        </is>
+      </c>
+    </row>
+    <row r="22" ht="15.9" customHeight="1" s="35" thickBot="1">
+      <c r="A22" s="48" t="n"/>
+      <c r="B22" s="50" t="n"/>
+      <c r="C22" s="33" t="inlineStr">
+        <is>
+          <t>1E</t>
+        </is>
+      </c>
+      <c r="D22" s="33" t="inlineStr">
+        <is>
+          <t>Activity 5</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="48" t="n"/>
+      <c r="B23" s="46" t="inlineStr">
+        <is>
+          <t>Trade 2</t>
+        </is>
+      </c>
+      <c r="C23" s="32" t="inlineStr">
+        <is>
+          <t>2A</t>
+        </is>
+      </c>
+      <c r="D23" s="32" t="inlineStr">
+        <is>
+          <t>Activity 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="48" t="n"/>
+      <c r="B24" s="48" t="n"/>
+      <c r="C24" s="31" t="inlineStr">
+        <is>
+          <t>2B</t>
+        </is>
+      </c>
+      <c r="D24" s="31" t="inlineStr">
+        <is>
+          <t>Activity 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="48" t="n"/>
+      <c r="B25" s="48" t="n"/>
+      <c r="C25" s="31" t="inlineStr">
+        <is>
+          <t>2C</t>
+        </is>
+      </c>
+      <c r="D25" s="31" t="inlineStr">
+        <is>
+          <t>Activity 3</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="48" t="n"/>
+      <c r="B26" s="48" t="n"/>
+      <c r="C26" s="31" t="inlineStr">
+        <is>
+          <t>2D</t>
+        </is>
+      </c>
+      <c r="D26" s="31" t="inlineStr">
+        <is>
+          <t>Activity 4</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="32" t="n"/>
+      <c r="B27" s="32" t="n"/>
+      <c r="C27" s="31" t="inlineStr">
+        <is>
+          <t>2E</t>
+        </is>
+      </c>
+      <c r="D27" s="31" t="inlineStr">
+        <is>
+          <t>Activity 5</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="6">
+    <mergeCell ref="A18:A27"/>
+    <mergeCell ref="B18:B22"/>
+    <mergeCell ref="AH2:AS2"/>
     <mergeCell ref="J1:AS1"/>
-    <mergeCell ref="AH2:AS2"/>
     <mergeCell ref="J2:AG2"/>
+    <mergeCell ref="B23:B27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3860,19 +4316,1507 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:AS27"/>
+  <sheetViews>
+    <sheetView zoomScale="69" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="N20" sqref="N20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15.6"/>
+  <cols>
+    <col width="8.046875" customWidth="1" style="35" min="2" max="2"/>
+    <col width="12.046875" bestFit="1" customWidth="1" style="35" min="3" max="3"/>
+    <col width="12.69921875" bestFit="1" customWidth="1" style="35" min="4" max="4"/>
+    <col width="5.34765625" bestFit="1" customWidth="1" style="35" min="9" max="9"/>
+    <col width="3.3984375" bestFit="1" customWidth="1" style="35" min="10" max="10"/>
+    <col width="3.84765625" bestFit="1" customWidth="1" style="35" min="11" max="11"/>
+    <col width="4.19921875" bestFit="1" customWidth="1" style="35" min="12" max="12"/>
+    <col width="3.59765625" bestFit="1" customWidth="1" style="35" min="13" max="13"/>
+    <col width="4.3984375" bestFit="1" customWidth="1" style="35" min="14" max="14"/>
+    <col width="3.59765625" bestFit="1" customWidth="1" style="35" min="15" max="15"/>
+    <col width="3.046875" bestFit="1" customWidth="1" style="35" min="16" max="16"/>
+    <col width="3.3984375" bestFit="1" customWidth="1" style="35" min="17" max="17"/>
+    <col width="3.84765625" bestFit="1" customWidth="1" style="35" min="18" max="18"/>
+    <col width="4.19921875" bestFit="1" customWidth="1" style="35" min="19" max="19"/>
+    <col width="3.59765625" bestFit="1" customWidth="1" style="35" min="20" max="20"/>
+    <col width="4.3984375" bestFit="1" customWidth="1" style="35" min="21" max="21"/>
+    <col width="3.59765625" bestFit="1" customWidth="1" style="35" min="22" max="22"/>
+    <col width="3.046875" bestFit="1" customWidth="1" style="35" min="23" max="23"/>
+    <col width="3.3984375" bestFit="1" customWidth="1" style="35" min="24" max="24"/>
+    <col width="3.84765625" bestFit="1" customWidth="1" style="35" min="25" max="25"/>
+    <col width="4.19921875" bestFit="1" customWidth="1" style="35" min="26" max="26"/>
+    <col width="3.59765625" bestFit="1" customWidth="1" style="35" min="27" max="27"/>
+    <col width="4.3984375" bestFit="1" customWidth="1" style="35" min="28" max="28"/>
+    <col width="3.59765625" bestFit="1" customWidth="1" style="35" min="29" max="29"/>
+    <col width="3.046875" bestFit="1" customWidth="1" style="35" min="30" max="30"/>
+    <col width="3.3984375" bestFit="1" customWidth="1" style="35" min="31" max="31"/>
+    <col width="3.84765625" bestFit="1" customWidth="1" style="35" min="32" max="32"/>
+    <col width="4.19921875" bestFit="1" customWidth="1" style="35" min="33" max="33"/>
+    <col width="3.59765625" bestFit="1" customWidth="1" style="35" min="34" max="34"/>
+    <col width="4.3984375" bestFit="1" customWidth="1" style="35" min="35" max="35"/>
+    <col width="3.59765625" bestFit="1" customWidth="1" style="35" min="36" max="36"/>
+    <col width="3.046875" bestFit="1" customWidth="1" style="35" min="37" max="37"/>
+    <col width="3.3984375" bestFit="1" customWidth="1" style="35" min="38" max="38"/>
+    <col width="3.84765625" bestFit="1" customWidth="1" style="35" min="39" max="39"/>
+    <col width="4.19921875" bestFit="1" customWidth="1" style="35" min="40" max="40"/>
+    <col width="3.59765625" bestFit="1" customWidth="1" style="35" min="41" max="41"/>
+    <col width="4.3984375" bestFit="1" customWidth="1" style="35" min="42" max="42"/>
+    <col width="3.59765625" bestFit="1" customWidth="1" style="35" min="43" max="43"/>
+    <col width="3.046875" bestFit="1" customWidth="1" style="35" min="44" max="44"/>
+    <col width="3.3984375" bestFit="1" customWidth="1" style="35" min="45" max="45"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="62.7" customHeight="1" s="35">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>CPM</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="AN1" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="AO1" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="AP1" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="AQ1" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="AR1" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="AS1" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Sep</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Sep</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Sep</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Sep</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>Sep</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>Sep</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>Sep</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>Sep</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>Sep</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>Sep</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>Sep</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>Sep</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>Sep</t>
+        </is>
+      </c>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>Sep</t>
+        </is>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>Sep</t>
+        </is>
+      </c>
+      <c r="X2" t="inlineStr">
+        <is>
+          <t>Sep</t>
+        </is>
+      </c>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>Sep</t>
+        </is>
+      </c>
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t>Sep</t>
+        </is>
+      </c>
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t>Sep</t>
+        </is>
+      </c>
+      <c r="AB2" t="inlineStr">
+        <is>
+          <t>Sep</t>
+        </is>
+      </c>
+      <c r="AC2" t="inlineStr">
+        <is>
+          <t>Sep</t>
+        </is>
+      </c>
+      <c r="AD2" t="inlineStr">
+        <is>
+          <t>Sep</t>
+        </is>
+      </c>
+      <c r="AE2" t="inlineStr">
+        <is>
+          <t>Sep</t>
+        </is>
+      </c>
+      <c r="AF2" t="inlineStr">
+        <is>
+          <t>Sep</t>
+        </is>
+      </c>
+      <c r="AG2" t="inlineStr">
+        <is>
+          <t>Sep</t>
+        </is>
+      </c>
+      <c r="AH2" t="inlineStr">
+        <is>
+          <t>Oct</t>
+        </is>
+      </c>
+      <c r="AI2" t="inlineStr">
+        <is>
+          <t>Oct</t>
+        </is>
+      </c>
+      <c r="AJ2" t="inlineStr">
+        <is>
+          <t>Oct</t>
+        </is>
+      </c>
+      <c r="AK2" t="inlineStr">
+        <is>
+          <t>Oct</t>
+        </is>
+      </c>
+      <c r="AL2" t="inlineStr">
+        <is>
+          <t>Oct</t>
+        </is>
+      </c>
+      <c r="AM2" t="inlineStr">
+        <is>
+          <t>Oct</t>
+        </is>
+      </c>
+      <c r="AN2" t="inlineStr">
+        <is>
+          <t>Oct</t>
+        </is>
+      </c>
+      <c r="AO2" t="inlineStr">
+        <is>
+          <t>Oct</t>
+        </is>
+      </c>
+      <c r="AP2" t="inlineStr">
+        <is>
+          <t>Oct</t>
+        </is>
+      </c>
+      <c r="AQ2" t="inlineStr">
+        <is>
+          <t>Oct</t>
+        </is>
+      </c>
+      <c r="AR2" t="inlineStr">
+        <is>
+          <t>Oct</t>
+        </is>
+      </c>
+      <c r="AS2" t="inlineStr">
+        <is>
+          <t>Oct</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>PM</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>LT</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>PM</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>LT</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>PM</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>PM</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>PM</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>06</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>07</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>08</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>09</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="Z3" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="AD3" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="AE3" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+      <c r="AF3" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+      <c r="AG3" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="AH3" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="AI3" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="AJ3" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="AK3" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
+      <c r="AL3" t="inlineStr">
+        <is>
+          <t>05</t>
+        </is>
+      </c>
+      <c r="AM3" t="inlineStr">
+        <is>
+          <t>06</t>
+        </is>
+      </c>
+      <c r="AN3" t="inlineStr">
+        <is>
+          <t>07</t>
+        </is>
+      </c>
+      <c r="AO3" t="inlineStr">
+        <is>
+          <t>08</t>
+        </is>
+      </c>
+      <c r="AP3" t="inlineStr">
+        <is>
+          <t>09</t>
+        </is>
+      </c>
+      <c r="AQ3" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="AR3" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="AS3" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Phase</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Location</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Trade</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Color</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Activity Code</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Activity Name</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Start</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Finish</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Fri</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Sat</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Sun</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>Mon</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>Tue</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>Wed</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>Thu</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>Fri</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>Sat</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>Sun</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>Mon</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>Tue</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>Wed</t>
+        </is>
+      </c>
+      <c r="V4" t="inlineStr">
+        <is>
+          <t>Thu</t>
+        </is>
+      </c>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>Fri</t>
+        </is>
+      </c>
+      <c r="X4" t="inlineStr">
+        <is>
+          <t>Sat</t>
+        </is>
+      </c>
+      <c r="Y4" t="inlineStr">
+        <is>
+          <t>Sun</t>
+        </is>
+      </c>
+      <c r="Z4" t="inlineStr">
+        <is>
+          <t>Mon</t>
+        </is>
+      </c>
+      <c r="AA4" t="inlineStr">
+        <is>
+          <t>Tue</t>
+        </is>
+      </c>
+      <c r="AB4" t="inlineStr">
+        <is>
+          <t>Wed</t>
+        </is>
+      </c>
+      <c r="AC4" t="inlineStr">
+        <is>
+          <t>Thu</t>
+        </is>
+      </c>
+      <c r="AD4" t="inlineStr">
+        <is>
+          <t>Fri</t>
+        </is>
+      </c>
+      <c r="AE4" t="inlineStr">
+        <is>
+          <t>Sat</t>
+        </is>
+      </c>
+      <c r="AF4" t="inlineStr">
+        <is>
+          <t>Sun</t>
+        </is>
+      </c>
+      <c r="AG4" t="inlineStr">
+        <is>
+          <t>Mon</t>
+        </is>
+      </c>
+      <c r="AH4" t="inlineStr">
+        <is>
+          <t>Tue</t>
+        </is>
+      </c>
+      <c r="AI4" t="inlineStr">
+        <is>
+          <t>Wed</t>
+        </is>
+      </c>
+      <c r="AJ4" t="inlineStr">
+        <is>
+          <t>Thu</t>
+        </is>
+      </c>
+      <c r="AK4" t="inlineStr">
+        <is>
+          <t>Fri</t>
+        </is>
+      </c>
+      <c r="AL4" t="inlineStr">
+        <is>
+          <t>Sat</t>
+        </is>
+      </c>
+      <c r="AM4" t="inlineStr">
+        <is>
+          <t>Sun</t>
+        </is>
+      </c>
+      <c r="AN4" t="inlineStr">
+        <is>
+          <t>Mon</t>
+        </is>
+      </c>
+      <c r="AO4" t="inlineStr">
+        <is>
+          <t>Tue</t>
+        </is>
+      </c>
+      <c r="AP4" t="inlineStr">
+        <is>
+          <t>Wed</t>
+        </is>
+      </c>
+      <c r="AQ4" t="inlineStr">
+        <is>
+          <t>Thu</t>
+        </is>
+      </c>
+      <c r="AR4" t="inlineStr">
+        <is>
+          <t>Fri</t>
+        </is>
+      </c>
+      <c r="AS4" t="inlineStr">
+        <is>
+          <t>Sat</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Phase 1</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Zone 1</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Trade 1</t>
+        </is>
+      </c>
+      <c r="D5" s="20" t="inlineStr">
+        <is>
+          <t>#8ED973</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>1A</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Activity 1</t>
+        </is>
+      </c>
+      <c r="G5" s="10" t="inlineStr">
+        <is>
+          <t>6-Sep-24</t>
+        </is>
+      </c>
+      <c r="H5" s="10" t="inlineStr">
+        <is>
+          <t>20-Sep-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Phase 1</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Zone 1</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Trade 2</t>
+        </is>
+      </c>
+      <c r="D6" s="21" t="inlineStr">
+        <is>
+          <t>#4D93D9</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>2A</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Activity 1</t>
+        </is>
+      </c>
+      <c r="G6" s="10" t="inlineStr">
+        <is>
+          <t>9-Sep-24</t>
+        </is>
+      </c>
+      <c r="H6" s="10" t="inlineStr">
+        <is>
+          <t>15-Sep-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Phase 1</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Zone 1</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Trade 1</t>
+        </is>
+      </c>
+      <c r="D7" s="20" t="inlineStr">
+        <is>
+          <t>#8ED973</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>1B</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Activity 2</t>
+        </is>
+      </c>
+      <c r="G7" s="10" t="inlineStr">
+        <is>
+          <t>30-Sep-24</t>
+        </is>
+      </c>
+      <c r="H7" s="10" t="inlineStr">
+        <is>
+          <t>5-Oct-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Phase 1</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Zone 1</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Trade 2</t>
+        </is>
+      </c>
+      <c r="D8" s="21" t="inlineStr">
+        <is>
+          <t>#4D93D9</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>2B</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Activity 2</t>
+        </is>
+      </c>
+      <c r="G8" s="10" t="inlineStr">
+        <is>
+          <t>16-Sep-24</t>
+        </is>
+      </c>
+      <c r="H8" s="10" t="inlineStr">
+        <is>
+          <t>19-Sep-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Phase 1</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Zone 1</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Trade 1</t>
+        </is>
+      </c>
+      <c r="D9" s="20" t="inlineStr">
+        <is>
+          <t>#8ED973</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>1C</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Activity 3</t>
+        </is>
+      </c>
+      <c r="G9" s="10" t="inlineStr">
+        <is>
+          <t>20-Sep-24</t>
+        </is>
+      </c>
+      <c r="H9" s="10" t="inlineStr">
+        <is>
+          <t>30-Sep-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Phase 1</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Zone 1</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Trade 2</t>
+        </is>
+      </c>
+      <c r="D10" s="21" t="inlineStr">
+        <is>
+          <t>#4D93D9</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>2C</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Activity 3</t>
+        </is>
+      </c>
+      <c r="G10" s="10" t="inlineStr">
+        <is>
+          <t>5-Oct-24</t>
+        </is>
+      </c>
+      <c r="H10" s="10" t="inlineStr">
+        <is>
+          <t>9-Oct-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Phase 1</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Zone 1</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Trade 1</t>
+        </is>
+      </c>
+      <c r="D11" s="20" t="inlineStr">
+        <is>
+          <t>#8ED973</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>1D</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Activity 4</t>
+        </is>
+      </c>
+      <c r="G11" s="10" t="inlineStr">
+        <is>
+          <t>28-Sep-24</t>
+        </is>
+      </c>
+      <c r="H11" s="10" t="inlineStr">
+        <is>
+          <t>12-Oct-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Phase 1</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Zone 1</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Trade 2</t>
+        </is>
+      </c>
+      <c r="D12" s="21" t="inlineStr">
+        <is>
+          <t>#4D93D9</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>2D</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Activity 4</t>
+        </is>
+      </c>
+      <c r="G12" s="10" t="inlineStr">
+        <is>
+          <t>5-Oct-24</t>
+        </is>
+      </c>
+      <c r="H12" s="10" t="inlineStr">
+        <is>
+          <t>7-Oct-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Phase 1</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Zone 1</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Trade 1</t>
+        </is>
+      </c>
+      <c r="D13" s="20" t="inlineStr">
+        <is>
+          <t>#8ED973</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>1E</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Activity 5</t>
+        </is>
+      </c>
+      <c r="G13" s="10" t="inlineStr">
+        <is>
+          <t>7-Oct-24</t>
+        </is>
+      </c>
+      <c r="H13" s="10" t="inlineStr">
+        <is>
+          <t>12-Oct-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Phase 1</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Zone 1</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Trade 2</t>
+        </is>
+      </c>
+      <c r="D14" s="21" t="inlineStr">
+        <is>
+          <t>#4D93D9</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>2E</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Activity 5</t>
+        </is>
+      </c>
+      <c r="G14" s="10" t="inlineStr">
+        <is>
+          <t>10-Oct-24</t>
+        </is>
+      </c>
+      <c r="H14" s="10" t="inlineStr">
+        <is>
+          <t>12-Oct-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="30" t="inlineStr">
+        <is>
+          <t>phase</t>
+        </is>
+      </c>
+      <c r="B17" s="30" t="inlineStr">
+        <is>
+          <t>trade</t>
+        </is>
+      </c>
+      <c r="C17" s="30" t="inlineStr">
+        <is>
+          <t>activity_code</t>
+        </is>
+      </c>
+      <c r="D17" s="30" t="inlineStr">
+        <is>
+          <t>activity_name</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="37" t="inlineStr">
+        <is>
+          <t>Phase 1</t>
+        </is>
+      </c>
+      <c r="B18" s="49" t="inlineStr">
+        <is>
+          <t>Trade 1</t>
+        </is>
+      </c>
+      <c r="C18" s="31" t="inlineStr">
+        <is>
+          <t>1A</t>
+        </is>
+      </c>
+      <c r="D18" s="31" t="inlineStr">
+        <is>
+          <t>Activity 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="48" t="n"/>
+      <c r="B19" s="48" t="n"/>
+      <c r="C19" s="31" t="inlineStr">
+        <is>
+          <t>1B</t>
+        </is>
+      </c>
+      <c r="D19" s="31" t="inlineStr">
+        <is>
+          <t>Activity 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="48" t="n"/>
+      <c r="B20" s="48" t="n"/>
+      <c r="C20" s="31" t="inlineStr">
+        <is>
+          <t>1C</t>
+        </is>
+      </c>
+      <c r="D20" s="31" t="inlineStr">
+        <is>
+          <t>Activity 3</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="48" t="n"/>
+      <c r="B21" s="48" t="n"/>
+      <c r="C21" s="31" t="inlineStr">
+        <is>
+          <t>1D</t>
+        </is>
+      </c>
+      <c r="D21" s="31" t="inlineStr">
+        <is>
+          <t>Activity 4</t>
+        </is>
+      </c>
+    </row>
+    <row r="22" ht="15.9" customHeight="1" s="35" thickBot="1">
+      <c r="A22" s="48" t="n"/>
+      <c r="B22" s="50" t="n"/>
+      <c r="C22" s="33" t="inlineStr">
+        <is>
+          <t>1E</t>
+        </is>
+      </c>
+      <c r="D22" s="33" t="inlineStr">
+        <is>
+          <t>Activity 5</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="48" t="n"/>
+      <c r="B23" s="46" t="inlineStr">
+        <is>
+          <t>Trade 2</t>
+        </is>
+      </c>
+      <c r="C23" s="32" t="inlineStr">
+        <is>
+          <t>2A</t>
+        </is>
+      </c>
+      <c r="D23" s="32" t="inlineStr">
+        <is>
+          <t>Activity 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="48" t="n"/>
+      <c r="B24" s="48" t="n"/>
+      <c r="C24" s="31" t="inlineStr">
+        <is>
+          <t>2B</t>
+        </is>
+      </c>
+      <c r="D24" s="31" t="inlineStr">
+        <is>
+          <t>Activity 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="48" t="n"/>
+      <c r="B25" s="48" t="n"/>
+      <c r="C25" s="31" t="inlineStr">
+        <is>
+          <t>2C</t>
+        </is>
+      </c>
+      <c r="D25" s="31" t="inlineStr">
+        <is>
+          <t>Activity 3</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="48" t="n"/>
+      <c r="B26" s="48" t="n"/>
+      <c r="C26" s="31" t="inlineStr">
+        <is>
+          <t>2D</t>
+        </is>
+      </c>
+      <c r="D26" s="31" t="inlineStr">
+        <is>
+          <t>Activity 4</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="32" t="n"/>
+      <c r="B27" s="32" t="n"/>
+      <c r="C27" s="31" t="inlineStr">
+        <is>
+          <t>2E</t>
+        </is>
+      </c>
+      <c r="D27" s="31" t="inlineStr">
+        <is>
+          <t>Activity 5</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A18:A27"/>
+    <mergeCell ref="B18:B22"/>
+    <mergeCell ref="B23:B27"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:AT33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11" defaultRowHeight="15.6" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
-    <col width="2.84765625" customWidth="1" min="9" max="9"/>
-    <col width="4" customWidth="1" min="10" max="46"/>
+    <col width="2.84765625" customWidth="1" style="35" min="9" max="9"/>
+    <col width="4" customWidth="1" style="35" min="10" max="46"/>
   </cols>
   <sheetData>
-    <row r="1" ht="62.1" customHeight="1">
+    <row r="1" ht="62.1" customHeight="1" s="35">
       <c r="A1" s="4" t="inlineStr">
         <is>
           <t>CPM</t>
@@ -4961,7 +6905,7 @@
         </is>
       </c>
     </row>
-    <row r="20" ht="62.7" customHeight="1">
+    <row r="20" ht="62.7" customHeight="1" s="35">
       <c r="G20" s="4" t="inlineStr">
         <is>
           <t>Flow Analysis</t>
@@ -5129,7 +7073,7 @@
           <t>Trade 1</t>
         </is>
       </c>
-      <c r="H22" s="20" t="n"/>
+      <c r="H22" s="18" t="n"/>
       <c r="J22" s="6" t="n">
         <v>45541</v>
       </c>
@@ -5793,7 +7737,7 @@
           <t>Trade 2</t>
         </is>
       </c>
-      <c r="H28" s="21" t="n"/>
+      <c r="H28" s="19" t="n"/>
       <c r="J28" s="8" t="n"/>
       <c r="K28" s="8" t="n"/>
       <c r="L28" s="8" t="n"/>

</xml_diff>